<commit_message>
fertig für den vormittag
</commit_message>
<xml_diff>
--- a/Auswertung_Studie.xlsx
+++ b/Auswertung_Studie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mweiler\Documents\GitHub\MMI_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCAAC79B-F387-42AC-A877-AD05025AC316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5F1833-0A03-47A8-9721-92FAC4172E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="0" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="73">
   <si>
     <t>Probandennr.</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>Hüfte</t>
-  </si>
-  <si>
-    <t>/</t>
   </si>
   <si>
     <t>Crosscountry</t>
@@ -493,6 +490,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -510,9 +510,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1322,7 +1319,7 @@
   <dimension ref="A1:BD27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,10 +1376,10 @@
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="30"/>
+      <c r="G1" s="31"/>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1392,74 +1389,74 @@
       <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="30"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="31"/>
       <c r="O1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="P1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="Q1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="31" t="s">
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="28" t="s">
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="29" t="s">
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="30"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="31"/>
       <c r="AK1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AL1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AM1" s="28" t="s">
+      <c r="AM1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
-      <c r="AQ1" s="28"/>
-      <c r="AR1" s="29" t="s">
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="AS1" s="28"/>
-      <c r="AT1" s="28"/>
-      <c r="AU1" s="28"/>
-      <c r="AV1" s="28"/>
-      <c r="AW1" s="30"/>
-      <c r="AX1" s="28" t="s">
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
+      <c r="AU1" s="29"/>
+      <c r="AV1" s="29"/>
+      <c r="AW1" s="31"/>
+      <c r="AX1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="AY1" s="28"/>
-      <c r="AZ1" s="28"/>
-      <c r="BA1" s="28"/>
-      <c r="BB1" s="28"/>
+      <c r="AY1" s="29"/>
+      <c r="AZ1" s="29"/>
+      <c r="BA1" s="29"/>
+      <c r="BB1" s="29"/>
       <c r="BC1" s="11" t="s">
         <v>18</v>
       </c>
@@ -1530,7 +1527,7 @@
         <v>68</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AC2" s="15" t="s">
         <v>57</v>
@@ -1571,7 +1568,7 @@
         <v>70</v>
       </c>
       <c r="AQ2" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AR2" s="14" t="s">
         <v>58</v>
@@ -2919,7 +2916,7 @@
       <c r="O15">
         <v>6</v>
       </c>
-      <c r="P15" s="34">
+      <c r="P15" s="28">
         <v>1.5</v>
       </c>
       <c r="Q15" s="4"/>
@@ -3247,7 +3244,7 @@
       <c r="O18">
         <v>10</v>
       </c>
-      <c r="P18" s="34">
+      <c r="P18" s="28">
         <v>3.5</v>
       </c>
       <c r="Q18" s="4" t="s">
@@ -3361,7 +3358,7 @@
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="V19" s="9"/>
       <c r="W19" s="4"/>
@@ -4294,6 +4291,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100C77408A9657D354AA2EA36B9C44B3D8B" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="35b7b4497c9b8f90ebc8a365f5a72516">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4073c1de-41dc-45a4-8e11-a80c309008b0" xmlns:ns3="013bd0e6-5a96-48c7-9517-6e2e630d5e76" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="10f9768fe295fb6f940ad6fb9ae135bb" ns2:_="" ns3:_="">
     <xsd:import namespace="4073c1de-41dc-45a4-8e11-a80c309008b0"/>
@@ -4486,15 +4492,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4507,6 +4504,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F9F41C6-20E3-42BB-83D6-45629D2E52BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3E58085-4949-4757-B14E-19CAFC17456B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4525,14 +4530,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F9F41C6-20E3-42BB-83D6-45629D2E52BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCA26C64-A250-4FCD-AAAE-4E8B17C6BE2C}">
   <ds:schemaRefs>

</xml_diff>